<commit_message>
changed www to docs to host on github
Will probably break next time it is run, update dir from www to docs
</commit_message>
<xml_diff>
--- a/bans.xlsx
+++ b/bans.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="780" yWindow="780" windowWidth="19425" windowHeight="10815" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2850" yWindow="2985" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -322,10 +322,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -390,7 +390,259 @@
         </is>
       </c>
     </row>
-    <row r="6"/>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SeokkSquirrel</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>afk</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>WiX21</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>afk</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Monkeygoberserk</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>afk</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Khabib_Time</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ak</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Enaxie</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>afk</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>BlizzlerButNot</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>afk</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>GRANDMAA</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>afk</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>gosling123</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>afk</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>UNDOMINABLE</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>throwing game</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>imasavage</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>afk</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>TrashOfCountsFamily</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>afk</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Mkool14</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>afk</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Polaris0</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>afk</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>z4ra0</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>afk</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Sephiroth_99</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>afk</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>khaiworld</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>afk</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>chug</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>afk</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>ice_dragon95</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>homophobia</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>BigPapaPanther</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>afk</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>N3xus</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>afk</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Ekizeel</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>afk</t>
+        </is>
+      </c>
+    </row>
+    <row r="27"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>